<commit_message>
Some updates to OT
</commit_message>
<xml_diff>
--- a/P3/Results/Data/Gips/Gypsum12g/Results/OTResults.xlsx
+++ b/P3/Results/Data/Gips/Gypsum12g/Results/OTResults.xlsx
@@ -1,67 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Filename</t>
-  </si>
-  <si>
-    <t>PSNR Ground checker diff Reference checker</t>
-  </si>
-  <si>
-    <t>PSNR Ground checker diff Enhanced checker</t>
-  </si>
-  <si>
-    <t>MBE Ground diff Reference</t>
-  </si>
-  <si>
-    <t>MBE Ground diff Enhanced</t>
-  </si>
-  <si>
-    <t>MBE Ground diff Dehazed</t>
-  </si>
-  <si>
-    <t>AG Ground</t>
-  </si>
-  <si>
-    <t>AG Reference</t>
-  </si>
-  <si>
-    <t>AG Enhanced</t>
-  </si>
-  <si>
-    <t>AG Dehazed</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -80,13 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -374,43 +407,449 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="73" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp75731.0_20242011_144931.png</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>12.76</v>
+      </c>
+      <c r="C2" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-23.51</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-5.81</v>
+      </c>
+      <c r="F2" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H2" t="n">
+        <v>4.14</v>
+      </c>
+      <c r="I2" t="n">
+        <v>16.98</v>
+      </c>
+      <c r="J2" t="n">
+        <v>6.91</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp112596.0_20242011_145005.png</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>12.14</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15.42</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-17.41</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-4.24</v>
+      </c>
+      <c r="F3" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>17.34</v>
+      </c>
+      <c r="J3" t="n">
+        <v>6.66</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light10_exp241011.0_20242011_145643.png</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>15.16</v>
+      </c>
+      <c r="C4" t="n">
+        <v>15.19</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-40.94</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-2.37</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10.87</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H4" t="n">
+        <v>7.34</v>
+      </c>
+      <c r="I4" t="n">
+        <v>17.88</v>
+      </c>
+      <c r="J4" t="n">
+        <v>9.869999999999999</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light5_exp229371.0_20242011_145511.png</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>13.87</v>
+      </c>
+      <c r="C5" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-24.06</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-4.44</v>
+      </c>
+      <c r="F5" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H5" t="n">
+        <v>6.16</v>
+      </c>
+      <c r="I5" t="n">
+        <v>19.87</v>
+      </c>
+      <c r="J5" t="n">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light10_exp79723.0_20242011_145354.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light5_exp120641.0_20242011_145421.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light10_exp179872.0_20242011_145732.png</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>15.06</v>
+      </c>
+      <c r="C8" t="n">
+        <v>14.89</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-36.03</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1.51</v>
+      </c>
+      <c r="F8" t="n">
+        <v>11.06</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H8" t="n">
+        <v>7.33</v>
+      </c>
+      <c r="I8" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="J8" t="n">
+        <v>10.06</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light5_exp200093.0_20242011_145809.png</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>14.96</v>
+      </c>
+      <c r="C9" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-23.44</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-2.69</v>
+      </c>
+      <c r="F9" t="n">
+        <v>15.02</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H9" t="n">
+        <v>6.48</v>
+      </c>
+      <c r="I9" t="n">
+        <v>19.72</v>
+      </c>
+      <c r="J9" t="n">
+        <v>8.369999999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp39957.0_20242011_145308.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp68580.0_20242011_145218.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp48796.0_20242011_145054.png</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>13.76</v>
+      </c>
+      <c r="C12" t="n">
+        <v>15.09</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-16.26</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1.38</v>
+      </c>
+      <c r="F12" t="n">
+        <v>17.24</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H12" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="I12" t="n">
+        <v>16.43</v>
+      </c>
+      <c r="J12" t="n">
+        <v>6.82</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp95117.0_20242011_145125.png</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>13.82</v>
+      </c>
+      <c r="C13" t="n">
+        <v>15.45</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-18.12</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-1.48</v>
+      </c>
+      <c r="F13" t="n">
+        <v>16.76</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H13" t="n">
+        <v>5.18</v>
+      </c>
+      <c r="I13" t="n">
+        <v>16.46</v>
+      </c>
+      <c r="J13" t="n">
+        <v>7.15</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightxUnderCam_exp231735.0_20242011_145948.png</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>13.78</v>
+      </c>
+      <c r="C14" t="n">
+        <v>14.92</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-18.29</v>
+      </c>
+      <c r="E14" t="n">
+        <v>10.51</v>
+      </c>
+      <c r="F14" t="n">
+        <v>11.57</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H14" t="n">
+        <v>7.36</v>
+      </c>
+      <c r="I14" t="n">
+        <v>9.65</v>
+      </c>
+      <c r="J14" t="n">
+        <v>8.970000000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp248261.0_20242011_145857.png</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>16.25</v>
+      </c>
+      <c r="C15" t="n">
+        <v>15.11</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-16.56</v>
+      </c>
+      <c r="E15" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="F15" t="n">
+        <v>14.15</v>
+      </c>
+      <c r="G15" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H15" t="n">
+        <v>6.82</v>
+      </c>
+      <c r="I15" t="n">
+        <v>11.55</v>
+      </c>
+      <c r="J15" t="n">
+        <v>8.19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>